<commit_message>
pie chart and design
</commit_message>
<xml_diff>
--- a/dataSources/monthData/dashSummary.xlsx
+++ b/dataSources/monthData/dashSummary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\VigneshD\repository\vsCode\KMDV-Dash\dataSources\monthData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AA6934D6-2B75-4AD2-894F-10328FA20C94}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69A7EA82-2C8C-49D8-8FD2-EA6C2FD2F6DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{0F5B5854-695B-4A75-A2C0-C1DAEEB6754A}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{0F5B5854-695B-4A75-A2C0-C1DAEEB6754A}"/>
   </bookViews>
   <sheets>
     <sheet name="Efforts" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="51">
   <si>
     <t>Project</t>
   </si>
@@ -173,6 +173,24 @@
   </si>
   <si>
     <t>Jul 24</t>
+  </si>
+  <si>
+    <t>Marketing</t>
+  </si>
+  <si>
+    <t>Finance</t>
+  </si>
+  <si>
+    <t>Investment</t>
+  </si>
+  <si>
+    <t>Business Operation</t>
+  </si>
+  <si>
+    <t>Client</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -751,7 +769,7 @@
   <dimension ref="A1:T22"/>
   <sheetViews>
     <sheetView zoomScale="87" workbookViewId="0">
-      <selection activeCell="K26" sqref="K26"/>
+      <selection activeCell="B2" sqref="B2:M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2003,10 +2021,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FDCE5C2A-DC0F-4E63-B0DF-E0CA59B2C830}">
-  <dimension ref="A1:T26"/>
+  <dimension ref="A1:T35"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" workbookViewId="0">
-      <selection activeCell="W12" sqref="W12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="E36" sqref="E36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -3239,133 +3257,686 @@
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" s="20"/>
+      <c r="B24" s="22"/>
+      <c r="C24" s="22"/>
+      <c r="D24" s="22"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+      <c r="G24" s="22"/>
+      <c r="H24" s="22"/>
+      <c r="I24" s="22"/>
+      <c r="J24" s="22"/>
+      <c r="K24" s="22"/>
+      <c r="L24" s="22"/>
+      <c r="M24" s="22"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
     </row>
     <row r="25" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
+      <c r="A25" s="20"/>
+      <c r="B25" s="22"/>
+      <c r="C25" s="22"/>
+      <c r="D25" s="22"/>
+      <c r="E25" s="22"/>
+      <c r="F25" s="22"/>
+      <c r="G25" s="22"/>
+      <c r="H25" s="22"/>
+      <c r="I25" s="22"/>
+      <c r="J25" s="22"/>
+      <c r="K25" s="22"/>
+      <c r="L25" s="22"/>
+      <c r="M25" s="22"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+    </row>
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A26" s="20"/>
+      <c r="B26" s="22"/>
+      <c r="C26" s="22"/>
+      <c r="D26" s="22"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="22"/>
+      <c r="G26" s="22"/>
+      <c r="H26" s="22"/>
+      <c r="I26" s="22"/>
+      <c r="J26" s="22"/>
+      <c r="K26" s="22"/>
+      <c r="L26" s="22"/>
+      <c r="M26" s="22"/>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+    </row>
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B27" s="5">
+        <f t="shared" ref="B27:T27" si="0">B12+B15</f>
+        <v>406.5</v>
+      </c>
+      <c r="C27" s="5">
+        <f t="shared" si="0"/>
+        <v>5360.25</v>
+      </c>
+      <c r="D27" s="5">
+        <f t="shared" si="0"/>
+        <v>4860</v>
+      </c>
+      <c r="E27" s="5">
+        <f t="shared" si="0"/>
+        <v>2728.5</v>
+      </c>
+      <c r="F27" s="5">
+        <f t="shared" si="0"/>
+        <v>3494.5</v>
+      </c>
+      <c r="G27" s="5">
+        <f t="shared" si="0"/>
+        <v>5647.5</v>
+      </c>
+      <c r="H27" s="5">
+        <f t="shared" si="0"/>
+        <v>8965.5</v>
+      </c>
+      <c r="I27" s="5">
+        <f t="shared" si="0"/>
+        <v>7978.5</v>
+      </c>
+      <c r="J27" s="5">
+        <f t="shared" si="0"/>
+        <v>8583</v>
+      </c>
+      <c r="K27" s="5">
+        <f t="shared" si="0"/>
+        <v>6993</v>
+      </c>
+      <c r="L27" s="5">
+        <f t="shared" si="0"/>
+        <v>8826</v>
+      </c>
+      <c r="M27" s="5">
+        <f t="shared" si="0"/>
+        <v>9825</v>
+      </c>
+      <c r="N27" s="5">
+        <f t="shared" si="0"/>
+        <v>406.5</v>
+      </c>
+      <c r="O27" s="5">
+        <f t="shared" si="0"/>
+        <v>5360.25</v>
+      </c>
+      <c r="P27" s="5">
+        <f t="shared" si="0"/>
+        <v>4860</v>
+      </c>
+      <c r="Q27" s="5">
+        <f t="shared" si="0"/>
+        <v>2728.5</v>
+      </c>
+      <c r="R27" s="5">
+        <f t="shared" si="0"/>
+        <v>3494.5</v>
+      </c>
+      <c r="S27" s="5">
+        <f t="shared" si="0"/>
+        <v>5647.5</v>
+      </c>
+      <c r="T27" s="5">
+        <f t="shared" si="0"/>
+        <v>8965.5</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A28" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B28" s="5">
+        <f>B16</f>
+        <v>0</v>
+      </c>
+      <c r="C28" s="5">
+        <f t="shared" ref="C28:T28" si="1">C16</f>
+        <v>0</v>
+      </c>
+      <c r="D28" s="5">
+        <f t="shared" si="1"/>
+        <v>1452</v>
+      </c>
+      <c r="E28" s="5">
+        <f t="shared" si="1"/>
+        <v>2178</v>
+      </c>
+      <c r="F28" s="5">
+        <f t="shared" si="1"/>
+        <v>1630.5</v>
+      </c>
+      <c r="G28" s="5">
+        <f t="shared" si="1"/>
+        <v>1785</v>
+      </c>
+      <c r="H28" s="5">
+        <f t="shared" si="1"/>
+        <v>1977</v>
+      </c>
+      <c r="I28" s="5">
+        <f t="shared" si="1"/>
+        <v>525</v>
+      </c>
+      <c r="J28" s="5">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="K28" s="5">
+        <f t="shared" si="1"/>
+        <v>360</v>
+      </c>
+      <c r="L28" s="5">
+        <f t="shared" si="1"/>
+        <v>1365</v>
+      </c>
+      <c r="M28" s="5">
+        <f t="shared" si="1"/>
+        <v>870</v>
+      </c>
+      <c r="N28" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="O28" s="5">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="P28" s="5">
+        <f t="shared" si="1"/>
+        <v>1452</v>
+      </c>
+      <c r="Q28" s="5">
+        <f t="shared" si="1"/>
+        <v>2178</v>
+      </c>
+      <c r="R28" s="5">
+        <f t="shared" si="1"/>
+        <v>1630.5</v>
+      </c>
+      <c r="S28" s="5">
+        <f t="shared" si="1"/>
+        <v>1785</v>
+      </c>
+      <c r="T28" s="5">
+        <f t="shared" si="1"/>
+        <v>1977</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A29" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B29" s="5">
+        <f>B20</f>
+        <v>0</v>
+      </c>
+      <c r="C29" s="5">
+        <f t="shared" ref="C29:T29" si="2">C20</f>
+        <v>0</v>
+      </c>
+      <c r="D29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="E29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="F29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="G29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="H29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="I29" s="5">
+        <f t="shared" si="2"/>
+        <v>4776</v>
+      </c>
+      <c r="J29" s="5">
+        <f t="shared" si="2"/>
+        <v>916.5</v>
+      </c>
+      <c r="K29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="L29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="M29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="N29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="O29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="P29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="Q29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="R29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="S29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+      <c r="T29" s="5">
+        <f t="shared" si="2"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B30" s="5">
+        <f t="shared" ref="B30:T30" si="3">B8+B19+B14+B5+B7+B10</f>
+        <v>21215</v>
+      </c>
+      <c r="C30" s="5">
+        <f t="shared" si="3"/>
+        <v>19983</v>
+      </c>
+      <c r="D30" s="5">
+        <f t="shared" si="3"/>
+        <v>22236</v>
+      </c>
+      <c r="E30" s="5">
+        <f t="shared" si="3"/>
+        <v>17361.75</v>
+      </c>
+      <c r="F30" s="5">
+        <f t="shared" si="3"/>
+        <v>20004.75</v>
+      </c>
+      <c r="G30" s="5">
+        <f t="shared" si="3"/>
+        <v>19473.75</v>
+      </c>
+      <c r="H30" s="5">
+        <f t="shared" si="3"/>
+        <v>23031</v>
+      </c>
+      <c r="I30" s="5">
+        <f t="shared" si="3"/>
+        <v>21377.25</v>
+      </c>
+      <c r="J30" s="5">
+        <f t="shared" si="3"/>
+        <v>18488.25</v>
+      </c>
+      <c r="K30" s="5">
+        <f t="shared" si="3"/>
+        <v>22569.75</v>
+      </c>
+      <c r="L30" s="5">
+        <f t="shared" si="3"/>
+        <v>20523</v>
+      </c>
+      <c r="M30" s="5">
+        <f t="shared" si="3"/>
+        <v>18222</v>
+      </c>
+      <c r="N30" s="5">
+        <f t="shared" si="3"/>
+        <v>21215</v>
+      </c>
+      <c r="O30" s="5">
+        <f t="shared" si="3"/>
+        <v>19983</v>
+      </c>
+      <c r="P30" s="5">
+        <f t="shared" si="3"/>
+        <v>22236</v>
+      </c>
+      <c r="Q30" s="5">
+        <f t="shared" si="3"/>
+        <v>17361.75</v>
+      </c>
+      <c r="R30" s="5">
+        <f t="shared" si="3"/>
+        <v>20004.75</v>
+      </c>
+      <c r="S30" s="5">
+        <f t="shared" si="3"/>
+        <v>19473.75</v>
+      </c>
+      <c r="T30" s="5">
+        <f t="shared" si="3"/>
+        <v>23031</v>
+      </c>
+    </row>
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A31" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B31" s="5">
+        <f t="shared" ref="B31:T31" si="4">B3+B22+B11</f>
+        <v>1782</v>
+      </c>
+      <c r="C31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="D31" s="5">
+        <f t="shared" si="4"/>
+        <v>1567.5</v>
+      </c>
+      <c r="E31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="F31" s="5">
+        <f t="shared" si="4"/>
+        <v>1320</v>
+      </c>
+      <c r="G31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="H31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="I31" s="5">
+        <f t="shared" si="4"/>
+        <v>1320</v>
+      </c>
+      <c r="J31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="K31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="L31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="M31" s="5">
+        <f t="shared" si="4"/>
+        <v>1698</v>
+      </c>
+      <c r="N31" s="5">
+        <f t="shared" si="4"/>
+        <v>1782</v>
+      </c>
+      <c r="O31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="P31" s="5">
+        <f t="shared" si="4"/>
+        <v>1567.5</v>
+      </c>
+      <c r="Q31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="R31" s="5">
+        <f t="shared" si="4"/>
+        <v>1320</v>
+      </c>
+      <c r="S31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+      <c r="T31" s="5">
+        <f t="shared" si="4"/>
+        <v>1056</v>
+      </c>
+    </row>
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A32" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B32" s="5">
+        <f>B9+B13+B6+B4+B21+B17+B18</f>
+        <v>15403.5</v>
+      </c>
+      <c r="C32" s="5">
+        <f t="shared" ref="C32:T32" si="5">C9+C13+C6+C4+C21+C17+C18</f>
+        <v>9792</v>
+      </c>
+      <c r="D32" s="5">
+        <f t="shared" si="5"/>
+        <v>7609.5</v>
+      </c>
+      <c r="E32" s="5">
+        <f t="shared" si="5"/>
+        <v>9405</v>
+      </c>
+      <c r="F32" s="5">
+        <f t="shared" si="5"/>
+        <v>7197.5</v>
+      </c>
+      <c r="G32" s="5">
+        <f t="shared" si="5"/>
+        <v>29468.25</v>
+      </c>
+      <c r="H32" s="5">
+        <f t="shared" si="5"/>
+        <v>22573.5</v>
+      </c>
+      <c r="I32" s="5">
+        <f t="shared" si="5"/>
+        <v>25963.5</v>
+      </c>
+      <c r="J32" s="5">
+        <f t="shared" si="5"/>
+        <v>19332</v>
+      </c>
+      <c r="K32" s="5">
+        <f t="shared" si="5"/>
+        <v>25789.5</v>
+      </c>
+      <c r="L32" s="5">
+        <f t="shared" si="5"/>
+        <v>21621</v>
+      </c>
+      <c r="M32" s="5">
+        <f t="shared" si="5"/>
+        <v>11268</v>
+      </c>
+      <c r="N32" s="5">
+        <f t="shared" si="5"/>
+        <v>15403.5</v>
+      </c>
+      <c r="O32" s="5">
+        <f t="shared" si="5"/>
+        <v>9792</v>
+      </c>
+      <c r="P32" s="5">
+        <f t="shared" si="5"/>
+        <v>7609.5</v>
+      </c>
+      <c r="Q32" s="5">
+        <f t="shared" si="5"/>
+        <v>9405</v>
+      </c>
+      <c r="R32" s="5">
+        <f t="shared" si="5"/>
+        <v>7197.5</v>
+      </c>
+      <c r="S32" s="5">
+        <f t="shared" si="5"/>
+        <v>29468.25</v>
+      </c>
+      <c r="T32" s="5">
+        <f t="shared" si="5"/>
+        <v>22573.5</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A33" s="20"/>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A34" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B25" s="5">
+      <c r="B34" s="5">
         <v>38807</v>
       </c>
-      <c r="C25" s="5">
+      <c r="C34" s="5">
         <v>36191.25</v>
       </c>
-      <c r="D25" s="5">
+      <c r="D34" s="5">
         <v>37725</v>
       </c>
-      <c r="E25" s="5">
+      <c r="E34" s="5">
         <v>32729.25</v>
       </c>
-      <c r="F25" s="5">
+      <c r="F34" s="5">
         <v>33647.25</v>
       </c>
-      <c r="G25" s="5">
+      <c r="G34" s="5">
         <v>57430.5</v>
       </c>
-      <c r="H25" s="5">
+      <c r="H34" s="5">
         <v>57603</v>
       </c>
-      <c r="I25" s="5">
+      <c r="I34" s="5">
         <v>61940.25</v>
       </c>
-      <c r="J25" s="5">
+      <c r="J34" s="5">
         <v>49245.75</v>
       </c>
-      <c r="K25" s="5">
+      <c r="K34" s="5">
         <v>56768.25</v>
       </c>
-      <c r="L25" s="5">
+      <c r="L34" s="5">
         <v>53391</v>
       </c>
-      <c r="M25" s="6">
+      <c r="M34" s="6">
         <v>41883</v>
       </c>
-      <c r="N25" s="5">
+      <c r="N34" s="5">
         <v>38807</v>
       </c>
-      <c r="O25" s="5">
+      <c r="O34" s="5">
         <v>36191.25</v>
       </c>
-      <c r="P25" s="5">
+      <c r="P34" s="5">
         <v>37725</v>
       </c>
-      <c r="Q25" s="5">
+      <c r="Q34" s="5">
         <v>32729.25</v>
       </c>
-      <c r="R25" s="5">
+      <c r="R34" s="5">
         <v>33647.25</v>
       </c>
-      <c r="S25" s="5">
+      <c r="S34" s="5">
         <v>57430.5</v>
       </c>
-      <c r="T25" s="5">
+      <c r="T34" s="5">
         <v>57603</v>
       </c>
     </row>
-    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A35" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B26" s="5">
+      <c r="B35" s="5">
         <v>62160</v>
       </c>
-      <c r="C26" s="5">
+      <c r="C35" s="5">
         <v>51659.530011587485</v>
       </c>
-      <c r="D26" s="5">
+      <c r="D35" s="5">
         <v>44160</v>
       </c>
-      <c r="E26" s="5">
+      <c r="E35" s="5">
         <v>47640</v>
       </c>
-      <c r="F26" s="5">
+      <c r="F35" s="5">
         <v>49175.999999999985</v>
       </c>
-      <c r="G26" s="5">
+      <c r="G35" s="5">
         <v>68206.569506830754</v>
       </c>
-      <c r="H26" s="5">
+      <c r="H35" s="5">
         <v>66654.000000000015</v>
       </c>
-      <c r="I26" s="5">
+      <c r="I35" s="5">
         <v>71148</v>
       </c>
-      <c r="J26" s="5">
+      <c r="J35" s="5">
         <v>66653.999999999985</v>
       </c>
-      <c r="K26" s="5">
+      <c r="K35" s="5">
         <v>63480</v>
       </c>
-      <c r="L26" s="5">
+      <c r="L35" s="5">
         <v>61110</v>
       </c>
-      <c r="M26" s="6">
+      <c r="M35" s="6">
         <v>54239.999999999993</v>
       </c>
-      <c r="N26" s="5">
+      <c r="N35" s="5">
         <v>62160</v>
       </c>
-      <c r="O26" s="5">
+      <c r="O35" s="5">
         <v>51659.530011587485</v>
       </c>
-      <c r="P26" s="5">
+      <c r="P35" s="5">
         <v>44160</v>
       </c>
-      <c r="Q26" s="5">
+      <c r="Q35" s="5">
         <v>47640</v>
       </c>
-      <c r="R26" s="5">
+      <c r="R35" s="5">
         <v>49175.999999999985</v>
       </c>
-      <c r="S26" s="5">
+      <c r="S35" s="5">
         <v>68206.569506830754</v>
       </c>
-      <c r="T26" s="5">
+      <c r="T35" s="5">
         <v>66654.000000000015</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -3373,7 +3944,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BF6A449-6462-40EC-A3DA-01359172B0CA}">
   <dimension ref="A1:T26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="T2" sqref="T2"/>
     </sheetView>
   </sheetViews>

</xml_diff>